<commit_message>
Fix error in conflict matrices between 31.2x2.1
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.5.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDF8AF6-95A4-4C55-B8D3-49CB7072538B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6330FB62-B544-4825-AC76-22C7E9E7E275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12915" yWindow="240" windowWidth="25770" windowHeight="20505" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -506,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336C9BFA-1A2F-4EA4-ABD9-F388641F4813}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -735,7 +735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -887,7 +889,7 @@
       <c r="S2" s="6">
         <v>38.200000000000003</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="7">
         <v>31.2</v>
       </c>
       <c r="U2" s="7">
@@ -2298,7 +2300,7 @@
       <c r="B19" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="7">
         <v>2.1</v>
       </c>
       <c r="D19" s="11">

</xml_diff>